<commit_message>
Version 1.6 - offenes Feedback
</commit_message>
<xml_diff>
--- a/LHIND_Mitbericht/GS/06 Kanal_fuer_Fachdaten-Eigenschaften_06092019_003443.xlsx
+++ b/LHIND_Mitbericht/GS/06 Kanal_fuer_Fachdaten-Eigenschaften_06092019_003443.xlsx
@@ -5,35 +5,33 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U720494\Downloads\Geschäftskonfiguration Mitberichtsverfahren BRA eigenes Departement\GS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U720494\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\33DJ7GCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216"/>
   </bookViews>
   <sheets>
     <sheet name="Inhalt" sheetId="2" r:id="rId1"/>
     <sheet name="Berechnet" sheetId="3" r:id="rId2"/>
     <sheet name="Datum_Uhrzeit" sheetId="4" r:id="rId3"/>
-    <sheet name="Ja_Nein" sheetId="8" r:id="rId4"/>
-    <sheet name="Katalog" sheetId="5" r:id="rId5"/>
-    <sheet name="Objektzeiger" sheetId="6" r:id="rId6"/>
-    <sheet name="Text" sheetId="7" r:id="rId7"/>
+    <sheet name="Katalog" sheetId="5" r:id="rId4"/>
+    <sheet name="Objektzeiger" sheetId="6" r:id="rId5"/>
+    <sheet name="Text" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Berechnet!$A$1:$S$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Datum_Uhrzeit!$A$1:$P$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Ja_Nein!$A$1:$O$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Katalog!$A$1:$P$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Objektzeiger!$A$1:$P$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Text!$A$1:$Q$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Katalog!$A$1:$P$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Objektzeiger!$A$1:$P$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Text!$A$1:$Q$2</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="158">
   <si>
     <t>Transportkanal</t>
   </si>
@@ -2008,46 +2006,6 @@
   </si>
   <si>
     <t>LHIND Gruppe (Bundesratsgeschäfte oder Geschäfte)</t>
-  </si>
-  <si>
-    <t>SpecialdataBooleanProperty</t>
-  </si>
-  <si>
-    <t>95f5ac4c-5469-4c5b-9419-4b2f8c5fc9c4</t>
-  </si>
-  <si>
-    <t>Ja_Nein</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Initialwert</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="1"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-ActaNova.Domain.Specialdata.Properties.SpecialdataBooleanProperty.DefaultValue</t>
-    </r>
-  </si>
-  <si>
-    <t>DE01B093-8730-4C07-86A7-5CE5A610908C</t>
-  </si>
-  <si>
-    <t>LHIND_Mitbericht_istFederfuehrung</t>
-  </si>
-  <si>
-    <t>Ist Federführung</t>
   </si>
 </sst>
 </file>
@@ -2102,7 +2060,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -2112,7 +2070,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2419,9 +2376,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
@@ -2433,10 +2390,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7"/>
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -2463,11 +2420,11 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -2502,63 +2459,52 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>160</v>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2858,117 +2804,6 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="39.109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="33" style="5" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="25.5546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" style="5" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="16" style="5" customWidth="1"/>
-    <col min="13" max="13" width="14" style="5" customWidth="1"/>
-    <col min="14" max="14" width="13" style="5" customWidth="1"/>
-    <col min="15" max="15" width="13.21875" style="5" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:O2"/>
-  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -3206,7 +3041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
@@ -3354,7 +3189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>

</xml_diff>